<commit_message>
Fixing some errors in testing files
</commit_message>
<xml_diff>
--- a/Battelle.EPA.WideAreaDecon.API.Tests/InputFiles/ParameterTests/ConstantDistribution.xlsx
+++ b/Battelle.EPA.WideAreaDecon.API.Tests/InputFiles/ParameterTests/ConstantDistribution.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\EPA\WideAreaDecon\WideAreaDecon\Battelle.EPA.WideAreaDecon.API.Tests\InputFiles\ParameterTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\EPA\WideAreaDecon\Battelle.EPA.WideAreaDecon.API.Tests\InputFiles\ParameterTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B82D3E5-9130-4B04-A7DB-BECAFFC8DFAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5AFEC4-18B0-4AB7-95A6-B4F4783007C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
-  <si>
-    <t>Internal</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -42,18 +36,6 @@
     <t>Distribution Type</t>
   </si>
   <si>
-    <t>Minimum</t>
-  </si>
-  <si>
-    <t>Maximum</t>
-  </si>
-  <si>
-    <t>Mean/Mode</t>
-  </si>
-  <si>
-    <t>Standard Deviation</t>
-  </si>
-  <si>
     <t>Constant</t>
   </si>
   <si>
@@ -79,6 +61,51 @@
   </si>
   <si>
     <t>The third test parameter</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Parameter 1</t>
+  </si>
+  <si>
+    <t>Parameter 2</t>
+  </si>
+  <si>
+    <t>Parameter 3</t>
+  </si>
+  <si>
+    <t>Parameter 4</t>
+  </si>
+  <si>
+    <t>Parameter 5</t>
+  </si>
+  <si>
+    <t>Parameter 6</t>
+  </si>
+  <si>
+    <t>Parameter 7</t>
+  </si>
+  <si>
+    <t>Lower Limit</t>
+  </si>
+  <si>
+    <t>Upper Limit</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Indoor;Underground;Outdoor</t>
+  </si>
+  <si>
+    <t>Indoor;Underground</t>
+  </si>
+  <si>
+    <t>Outdoor</t>
   </si>
 </sst>
 </file>
@@ -396,104 +423,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>4</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>4</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>